<commit_message>
this notebook will complete the 4 tables at the back of the assignment packet
</commit_message>
<xml_diff>
--- a/data/nh_data_oct_18.xlsx
+++ b/data/nh_data_oct_18.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kris/GitHub/fall_2024_forested_landscape/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AF5335-FB30-AF40-90BA-386731BFC5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D61D64-E75C-1143-A176-A0A332FA18D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1665,7 +1665,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>